<commit_message>
+ BOM * Switch to newer KiCAD
</commit_message>
<xml_diff>
--- a/UsbHost_hw/UsbHostBOM.xlsx
+++ b/UsbHost_hw/UsbHostBOM.xlsx
@@ -566,7 +566,7 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -633,6 +633,9 @@
       <c r="D3">
         <v>4</v>
       </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -647,6 +650,9 @@
       <c r="D4">
         <v>1</v>
       </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -661,6 +667,9 @@
       <c r="D5">
         <v>1</v>
       </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -675,6 +684,9 @@
       <c r="D6">
         <v>10</v>
       </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -689,6 +701,9 @@
       <c r="D7">
         <v>2</v>
       </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -703,6 +718,9 @@
       <c r="D8">
         <v>4</v>
       </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -717,6 +735,9 @@
       <c r="D9">
         <v>0</v>
       </c>
+      <c r="F9">
+        <v>17</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -732,7 +753,7 @@
         <v>1</v>
       </c>
       <c r="F10">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G10">
         <v>3</v>
@@ -751,6 +772,9 @@
       <c r="D11">
         <v>1</v>
       </c>
+      <c r="F11">
+        <v>164</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -765,6 +789,9 @@
       <c r="D12">
         <v>1</v>
       </c>
+      <c r="F12">
+        <v>211</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -779,6 +806,9 @@
       <c r="D13">
         <v>1</v>
       </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -813,6 +843,9 @@
       <c r="D15">
         <v>3</v>
       </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -827,6 +860,9 @@
       <c r="D16">
         <v>2</v>
       </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -842,7 +878,7 @@
         <v>1</v>
       </c>
       <c r="F17">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="G17">
         <v>2</v>
@@ -861,6 +897,9 @@
       <c r="D18">
         <v>1</v>
       </c>
+      <c r="F18">
+        <v>2</v>
+      </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -878,6 +917,9 @@
       <c r="E19">
         <v>6</v>
       </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -892,6 +934,9 @@
       <c r="D20">
         <v>1</v>
       </c>
+      <c r="F20">
+        <v>47</v>
+      </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
@@ -925,6 +970,9 @@
       </c>
       <c r="D22">
         <v>1</v>
+      </c>
+      <c r="F22">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>